<commit_message>
final report of pattern recognition assignment
</commit_message>
<xml_diff>
--- a/pattern recognition/density confusion matrix.xlsx
+++ b/pattern recognition/density confusion matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ponti\Documents\GitHub\DataMining\pattern recognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B673DD-8220-4663-95D6-786477E6D632}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD2F866-A8C3-4479-A338-1549697A7CA0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1111,7 +1111,7 @@
   <dimension ref="A1:Z70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F46" workbookViewId="0">
-      <selection activeCell="Q75" sqref="Q75"/>
+      <selection activeCell="H59" sqref="H59:S70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2600,7 +2600,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K59" s="6">
         <v>2</v>
@@ -2635,38 +2635,38 @@
         <v>0</v>
       </c>
       <c r="I60" s="19">
-        <v>3468</v>
+        <v>3438</v>
       </c>
       <c r="J60" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K60" s="20">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="L60" s="20">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="M60" s="20">
         <v>9</v>
       </c>
       <c r="N60" s="20">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="O60" s="20">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="P60" s="20">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="Q60" s="20">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="R60" s="21">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="S60">
         <f>SUM(I60:R60)</f>
-        <v>3642</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="61" spans="8:19" x14ac:dyDescent="0.35">
@@ -2674,38 +2674,38 @@
         <v>1</v>
       </c>
       <c r="I61" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J61" s="1">
-        <v>3981</v>
+        <v>3979</v>
       </c>
       <c r="K61" s="1">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="L61" s="1">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="M61" s="1">
         <v>26</v>
       </c>
       <c r="N61" s="1">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="O61" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P61" s="1">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q61" s="1">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="R61" s="2">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="S61">
         <f t="shared" ref="S61:S70" si="6">SUM(I61:R61)</f>
-        <v>4316</v>
+        <v>4271</v>
       </c>
     </row>
     <row r="62" spans="8:19" x14ac:dyDescent="0.35">
@@ -2713,38 +2713,38 @@
         <v>2</v>
       </c>
       <c r="I62" s="22">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="J62" s="1">
+        <v>29</v>
+      </c>
+      <c r="K62" s="1">
+        <v>3228</v>
+      </c>
+      <c r="L62" s="1">
+        <v>101</v>
+      </c>
+      <c r="M62" s="1">
         <v>19</v>
       </c>
-      <c r="K62" s="1">
-        <v>3149</v>
-      </c>
-      <c r="L62" s="1">
-        <v>103</v>
-      </c>
-      <c r="M62" s="1">
-        <v>25</v>
-      </c>
       <c r="N62" s="1">
+        <v>41</v>
+      </c>
+      <c r="O62" s="1">
         <v>35</v>
       </c>
-      <c r="O62" s="1">
-        <v>51</v>
-      </c>
       <c r="P62" s="1">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="Q62" s="1">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="R62" s="2">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="S62">
         <f t="shared" si="6"/>
-        <v>3542</v>
+        <v>3599</v>
       </c>
     </row>
     <row r="63" spans="8:19" x14ac:dyDescent="0.35">
@@ -2752,38 +2752,38 @@
         <v>3</v>
       </c>
       <c r="I63" s="22">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J63" s="1">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="K63" s="1">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="L63" s="1">
-        <v>3298</v>
+        <v>3378</v>
       </c>
       <c r="M63" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N63" s="1">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="O63" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P63" s="1">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="Q63" s="1">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="R63" s="2">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="S63">
         <f t="shared" si="6"/>
-        <v>3806</v>
+        <v>3828</v>
       </c>
     </row>
     <row r="64" spans="8:19" x14ac:dyDescent="0.35">
@@ -2791,38 +2791,38 @@
         <v>4</v>
       </c>
       <c r="I64" s="22">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J64" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K64" s="1">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="L64" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="M64" s="1">
-        <v>3238</v>
+        <v>3296</v>
       </c>
       <c r="N64" s="1">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="O64" s="1">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="P64" s="1">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="Q64" s="1">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="R64" s="2">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="S64">
         <f t="shared" si="6"/>
-        <v>3639</v>
+        <v>3770</v>
       </c>
     </row>
     <row r="65" spans="8:19" x14ac:dyDescent="0.35">
@@ -2830,38 +2830,38 @@
         <v>5</v>
       </c>
       <c r="I65" s="22">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="J65" s="1">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K65" s="1">
         <v>24</v>
       </c>
       <c r="L65" s="1">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="M65" s="1">
+        <v>14</v>
+      </c>
+      <c r="N65" s="1">
+        <v>2795</v>
+      </c>
+      <c r="O65" s="1">
+        <v>48</v>
+      </c>
+      <c r="P65" s="1">
         <v>11</v>
       </c>
-      <c r="N65" s="1">
-        <v>2792</v>
-      </c>
-      <c r="O65" s="1">
-        <v>62</v>
-      </c>
-      <c r="P65" s="1">
-        <v>9</v>
-      </c>
       <c r="Q65" s="1">
-        <v>128</v>
+        <v>89</v>
       </c>
       <c r="R65" s="2">
         <v>31</v>
       </c>
       <c r="S65">
         <f t="shared" si="6"/>
-        <v>3329</v>
+        <v>3231</v>
       </c>
     </row>
     <row r="66" spans="8:19" x14ac:dyDescent="0.35">
@@ -2869,38 +2869,38 @@
         <v>6</v>
       </c>
       <c r="I66" s="22">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="J66" s="1">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K66" s="1">
-        <v>86</v>
+        <v>39</v>
       </c>
       <c r="L66" s="1">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="M66" s="1">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="N66" s="1">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="O66" s="1">
-        <v>3438</v>
+        <v>3407</v>
       </c>
       <c r="P66" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Q66" s="1">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="R66" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="S66">
         <f t="shared" si="6"/>
-        <v>3760</v>
+        <v>3724</v>
       </c>
     </row>
     <row r="67" spans="8:19" x14ac:dyDescent="0.35">
@@ -2908,38 +2908,38 @@
         <v>7</v>
       </c>
       <c r="I67" s="22">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J67" s="1">
+        <v>10</v>
+      </c>
+      <c r="K67" s="1">
+        <v>67</v>
+      </c>
+      <c r="L67" s="1">
+        <v>45</v>
+      </c>
+      <c r="M67" s="1">
+        <v>5</v>
+      </c>
+      <c r="N67" s="1">
+        <v>39</v>
+      </c>
+      <c r="O67" s="1">
+        <v>1</v>
+      </c>
+      <c r="P67" s="1">
+        <v>3533</v>
+      </c>
+      <c r="Q67" s="1">
         <v>13</v>
       </c>
-      <c r="K67" s="1">
-        <v>71</v>
-      </c>
-      <c r="L67" s="1">
-        <v>57</v>
-      </c>
-      <c r="M67" s="1">
-        <v>15</v>
-      </c>
-      <c r="N67" s="1">
-        <v>33</v>
-      </c>
-      <c r="O67" s="1">
-        <v>10</v>
-      </c>
-      <c r="P67" s="1">
-        <v>3452</v>
-      </c>
-      <c r="Q67" s="1">
-        <v>12</v>
-      </c>
       <c r="R67" s="2">
-        <v>152</v>
+        <v>83</v>
       </c>
       <c r="S67">
         <f t="shared" si="6"/>
-        <v>3827</v>
+        <v>3807</v>
       </c>
     </row>
     <row r="68" spans="8:19" x14ac:dyDescent="0.35">
@@ -2947,38 +2947,38 @@
         <v>8</v>
       </c>
       <c r="I68" s="22">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J68" s="1">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K68" s="1">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="L68" s="1">
         <v>63</v>
       </c>
       <c r="M68" s="1">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N68" s="1">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="O68" s="1">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="P68" s="1">
         <v>17</v>
       </c>
       <c r="Q68" s="1">
-        <v>2974</v>
+        <v>3083</v>
       </c>
       <c r="R68" s="2">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="S68">
         <f t="shared" si="6"/>
-        <v>3408</v>
+        <v>3456</v>
       </c>
     </row>
     <row r="69" spans="8:19" x14ac:dyDescent="0.35">
@@ -2986,38 +2986,38 @@
         <v>9</v>
       </c>
       <c r="I69" s="23">
+        <v>7</v>
+      </c>
+      <c r="J69" s="3">
         <v>4</v>
       </c>
-      <c r="J69" s="3">
-        <v>2</v>
-      </c>
       <c r="K69" s="3">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="L69" s="3">
         <v>51</v>
       </c>
       <c r="M69" s="3">
-        <v>193</v>
+        <v>120</v>
       </c>
       <c r="N69" s="3">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="O69" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P69" s="3">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="Q69" s="3">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="R69" s="4">
-        <v>3171</v>
+        <v>3263</v>
       </c>
       <c r="S69">
         <f t="shared" si="6"/>
-        <v>3731</v>
+        <v>3698</v>
       </c>
     </row>
     <row r="70" spans="8:19" x14ac:dyDescent="0.35">
@@ -3026,43 +3026,43 @@
       </c>
       <c r="I70">
         <f>SUM(I60:I69)</f>
-        <v>3641</v>
+        <v>3652</v>
       </c>
       <c r="J70">
         <f t="shared" ref="J70:R70" si="7">SUM(J60:J69)</f>
-        <v>4118</v>
+        <v>4115</v>
       </c>
       <c r="K70">
         <f t="shared" si="7"/>
-        <v>3653</v>
+        <v>3643</v>
       </c>
       <c r="L70">
         <f t="shared" si="7"/>
-        <v>3832</v>
+        <v>3848</v>
       </c>
       <c r="M70">
         <f t="shared" si="7"/>
-        <v>3598</v>
+        <v>3575</v>
       </c>
       <c r="N70">
         <f t="shared" si="7"/>
-        <v>3349</v>
+        <v>3353</v>
       </c>
       <c r="O70">
         <f t="shared" si="7"/>
-        <v>3669</v>
+        <v>3653</v>
       </c>
       <c r="P70">
         <f t="shared" si="7"/>
-        <v>3863</v>
+        <v>3893</v>
       </c>
       <c r="Q70">
         <f t="shared" si="7"/>
-        <v>3578</v>
+        <v>3575</v>
       </c>
       <c r="R70">
         <f t="shared" si="7"/>
-        <v>3699</v>
+        <v>3693</v>
       </c>
       <c r="S70">
         <f t="shared" si="6"/>

</xml_diff>